<commit_message>
update API , task #19898, #1990->#19912
</commit_message>
<xml_diff>
--- a/doc/backend/api/TRN-MiniBlog_API-Specification_NguyenLeQuocViet.xlsx
+++ b/doc/backend/api/TRN-MiniBlog_API-Specification_NguyenLeQuocViet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="640" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="23" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="API List" sheetId="46" r:id="rId5"/>
     <sheet name="Create user" sheetId="34" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="247">
   <si>
     <t>Description</t>
   </si>
@@ -696,6 +696,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>response</t>
     </r>
@@ -754,6 +755,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>mail address</t>
     </r>
@@ -762,6 +764,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>.</t>
     </r>
@@ -773,6 +776,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Create </t>
     </r>
@@ -782,6 +786,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">User </t>
     </r>
@@ -791,6 +796,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>A</t>
     </r>
@@ -800,6 +806,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>ccount</t>
     </r>
@@ -842,13 +849,19 @@
   </si>
   <si>
     <t>nguyen.viet@mulodo.com</t>
+  </si>
+  <si>
+    <t>Database do not have data</t>
+  </si>
+  <si>
+    <t>{Should input with true data}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="35">
+  <fonts count="37">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -890,6 +903,7 @@
       <sz val="18"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -897,18 +911,21 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -916,18 +933,21 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF963634"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -939,6 +959,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -951,38 +972,46 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1030,27 +1059,44 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF502EDE"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1709,7 +1755,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="247">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2116,29 +2162,73 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2150,44 +2240,6 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2216,6 +2268,21 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="10" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="242" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -2228,54 +2295,33 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="11" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="10" xfId="243" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="12" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="13" xfId="243" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="242" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2315,14 +2361,8 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2339,6 +2379,9 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2353,6 +2396,27 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="411">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2769,6 +2833,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF502EDE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4552,297 +4621,297 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="43" customFormat="1" ht="15.75">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="201" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="173" t="s">
+      <c r="B1" s="202"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
-      <c r="H1" s="174"/>
-      <c r="I1" s="174"/>
-      <c r="J1" s="174"/>
-      <c r="K1" s="175" t="s">
+      <c r="E1" s="205"/>
+      <c r="F1" s="205"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="205"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
+      <c r="K1" s="209" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="176"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="178" t="s">
+      <c r="L1" s="210"/>
+      <c r="M1" s="211"/>
+      <c r="N1" s="191" t="s">
         <v>155</v>
       </c>
-      <c r="O1" s="179"/>
-      <c r="P1" s="179"/>
-      <c r="Q1" s="179"/>
-      <c r="R1" s="179"/>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="181" t="s">
+      <c r="O1" s="192"/>
+      <c r="P1" s="192"/>
+      <c r="Q1" s="192"/>
+      <c r="R1" s="192"/>
+      <c r="S1" s="192"/>
+      <c r="T1" s="192"/>
+      <c r="U1" s="193"/>
+      <c r="V1" s="212" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="182"/>
-      <c r="X1" s="182"/>
-      <c r="Y1" s="182"/>
-      <c r="Z1" s="182"/>
-      <c r="AA1" s="182"/>
-      <c r="AB1" s="182"/>
-      <c r="AC1" s="182"/>
-      <c r="AD1" s="183"/>
+      <c r="W1" s="213"/>
+      <c r="X1" s="213"/>
+      <c r="Y1" s="213"/>
+      <c r="Z1" s="213"/>
+      <c r="AA1" s="213"/>
+      <c r="AB1" s="213"/>
+      <c r="AC1" s="213"/>
+      <c r="AD1" s="214"/>
     </row>
     <row r="2" spans="1:30" s="43" customFormat="1" ht="15.75">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="201" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="173" t="s">
+      <c r="B2" s="202"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="204" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="174"/>
-      <c r="J2" s="174"/>
-      <c r="K2" s="187" t="s">
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="205"/>
+      <c r="I2" s="205"/>
+      <c r="J2" s="205"/>
+      <c r="K2" s="186" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="188"/>
-      <c r="M2" s="189"/>
-      <c r="N2" s="199" t="s">
+      <c r="L2" s="187"/>
+      <c r="M2" s="188"/>
+      <c r="N2" s="206" t="s">
         <v>233</v>
       </c>
-      <c r="O2" s="200"/>
-      <c r="P2" s="200"/>
-      <c r="Q2" s="200"/>
-      <c r="R2" s="200"/>
-      <c r="S2" s="200"/>
-      <c r="T2" s="200"/>
-      <c r="U2" s="201"/>
-      <c r="V2" s="184" t="s">
+      <c r="O2" s="207"/>
+      <c r="P2" s="207"/>
+      <c r="Q2" s="207"/>
+      <c r="R2" s="207"/>
+      <c r="S2" s="207"/>
+      <c r="T2" s="207"/>
+      <c r="U2" s="208"/>
+      <c r="V2" s="183" t="s">
         <v>159</v>
       </c>
-      <c r="W2" s="185"/>
-      <c r="X2" s="186"/>
-      <c r="Y2" s="184" t="s">
+      <c r="W2" s="184"/>
+      <c r="X2" s="185"/>
+      <c r="Y2" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="185"/>
-      <c r="AA2" s="186"/>
-      <c r="AB2" s="184" t="s">
+      <c r="Z2" s="184"/>
+      <c r="AA2" s="185"/>
+      <c r="AB2" s="183" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="185"/>
-      <c r="AD2" s="186"/>
+      <c r="AC2" s="184"/>
+      <c r="AD2" s="185"/>
     </row>
     <row r="3" spans="1:30" s="43" customFormat="1" ht="15.75">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="186" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="188"/>
-      <c r="C3" s="189"/>
-      <c r="D3" s="190" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="188"/>
+      <c r="D3" s="189" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="191"/>
-      <c r="F3" s="191"/>
-      <c r="G3" s="191"/>
-      <c r="H3" s="191"/>
-      <c r="I3" s="191"/>
-      <c r="J3" s="191"/>
-      <c r="K3" s="187" t="s">
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="186" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="188"/>
-      <c r="M3" s="189"/>
-      <c r="N3" s="178" t="s">
+      <c r="L3" s="187"/>
+      <c r="M3" s="188"/>
+      <c r="N3" s="191" t="s">
         <v>158</v>
       </c>
-      <c r="O3" s="179"/>
-      <c r="P3" s="179"/>
-      <c r="Q3" s="179"/>
-      <c r="R3" s="179"/>
-      <c r="S3" s="179"/>
-      <c r="T3" s="179"/>
-      <c r="U3" s="180"/>
-      <c r="V3" s="192"/>
-      <c r="W3" s="193"/>
-      <c r="X3" s="194"/>
-      <c r="Y3" s="195"/>
-      <c r="Z3" s="196"/>
-      <c r="AA3" s="197"/>
-      <c r="AB3" s="198"/>
-      <c r="AC3" s="196"/>
-      <c r="AD3" s="197"/>
+      <c r="O3" s="192"/>
+      <c r="P3" s="192"/>
+      <c r="Q3" s="192"/>
+      <c r="R3" s="192"/>
+      <c r="S3" s="192"/>
+      <c r="T3" s="192"/>
+      <c r="U3" s="193"/>
+      <c r="V3" s="194"/>
+      <c r="W3" s="195"/>
+      <c r="X3" s="196"/>
+      <c r="Y3" s="197"/>
+      <c r="Z3" s="198"/>
+      <c r="AA3" s="199"/>
+      <c r="AB3" s="200"/>
+      <c r="AC3" s="198"/>
+      <c r="AD3" s="199"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:30" ht="16.5" thickBot="1">
-      <c r="B8" s="214" t="s">
+      <c r="B8" s="181" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="214"/>
-      <c r="D8" s="214"/>
-      <c r="E8" s="214"/>
-      <c r="F8" s="214" t="s">
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="214"/>
-      <c r="H8" s="214" t="s">
+      <c r="G8" s="181"/>
+      <c r="H8" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="214"/>
-      <c r="J8" s="214"/>
-      <c r="K8" s="214" t="s">
+      <c r="I8" s="181"/>
+      <c r="J8" s="181"/>
+      <c r="K8" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="214"/>
-      <c r="M8" s="214"/>
-      <c r="N8" s="214"/>
-      <c r="O8" s="214"/>
-      <c r="P8" s="214"/>
-      <c r="Q8" s="214"/>
-      <c r="R8" s="214"/>
-      <c r="S8" s="214"/>
-      <c r="T8" s="214"/>
-      <c r="U8" s="214"/>
-      <c r="V8" s="214"/>
-      <c r="W8" s="214"/>
-      <c r="X8" s="214" t="s">
+      <c r="L8" s="181"/>
+      <c r="M8" s="181"/>
+      <c r="N8" s="181"/>
+      <c r="O8" s="181"/>
+      <c r="P8" s="181"/>
+      <c r="Q8" s="181"/>
+      <c r="R8" s="181"/>
+      <c r="S8" s="181"/>
+      <c r="T8" s="181"/>
+      <c r="U8" s="181"/>
+      <c r="V8" s="181"/>
+      <c r="W8" s="181"/>
+      <c r="X8" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="Y8" s="214"/>
-      <c r="Z8" s="214"/>
-      <c r="AA8" s="214"/>
-      <c r="AB8" s="214"/>
-      <c r="AC8" s="214"/>
+      <c r="Y8" s="181"/>
+      <c r="Z8" s="181"/>
+      <c r="AA8" s="181"/>
+      <c r="AB8" s="181"/>
+      <c r="AC8" s="181"/>
     </row>
     <row r="9" spans="1:30">
-      <c r="B9" s="202" t="s">
+      <c r="B9" s="182" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="203"/>
-      <c r="D9" s="203"/>
-      <c r="E9" s="204"/>
-      <c r="F9" s="205" t="s">
+      <c r="C9" s="171"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="173" t="s">
         <v>154</v>
       </c>
-      <c r="G9" s="206"/>
-      <c r="H9" s="207"/>
-      <c r="I9" s="203"/>
-      <c r="J9" s="204"/>
-      <c r="K9" s="208"/>
-      <c r="L9" s="209"/>
-      <c r="M9" s="209"/>
-      <c r="N9" s="209"/>
-      <c r="O9" s="209"/>
-      <c r="P9" s="209"/>
-      <c r="Q9" s="209"/>
-      <c r="R9" s="209"/>
-      <c r="S9" s="209"/>
-      <c r="T9" s="209"/>
-      <c r="U9" s="209"/>
-      <c r="V9" s="209"/>
-      <c r="W9" s="210"/>
-      <c r="X9" s="211"/>
-      <c r="Y9" s="212"/>
-      <c r="Z9" s="212"/>
-      <c r="AA9" s="212"/>
-      <c r="AB9" s="212"/>
-      <c r="AC9" s="213"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="170"/>
+      <c r="I9" s="171"/>
+      <c r="J9" s="172"/>
+      <c r="K9" s="175"/>
+      <c r="L9" s="176"/>
+      <c r="M9" s="176"/>
+      <c r="N9" s="176"/>
+      <c r="O9" s="176"/>
+      <c r="P9" s="176"/>
+      <c r="Q9" s="176"/>
+      <c r="R9" s="176"/>
+      <c r="S9" s="176"/>
+      <c r="T9" s="176"/>
+      <c r="U9" s="176"/>
+      <c r="V9" s="176"/>
+      <c r="W9" s="177"/>
+      <c r="X9" s="178"/>
+      <c r="Y9" s="179"/>
+      <c r="Z9" s="179"/>
+      <c r="AA9" s="179"/>
+      <c r="AB9" s="179"/>
+      <c r="AC9" s="180"/>
     </row>
     <row r="10" spans="1:30">
-      <c r="B10" s="207"/>
-      <c r="C10" s="203"/>
-      <c r="D10" s="203"/>
-      <c r="E10" s="204"/>
-      <c r="F10" s="205"/>
-      <c r="G10" s="206"/>
-      <c r="H10" s="207"/>
-      <c r="I10" s="203"/>
-      <c r="J10" s="204"/>
-      <c r="K10" s="208"/>
-      <c r="L10" s="209"/>
-      <c r="M10" s="209"/>
-      <c r="N10" s="209"/>
-      <c r="O10" s="209"/>
-      <c r="P10" s="209"/>
-      <c r="Q10" s="209"/>
-      <c r="R10" s="209"/>
-      <c r="S10" s="209"/>
-      <c r="T10" s="209"/>
-      <c r="U10" s="209"/>
-      <c r="V10" s="209"/>
-      <c r="W10" s="210"/>
-      <c r="X10" s="211"/>
-      <c r="Y10" s="212"/>
-      <c r="Z10" s="212"/>
-      <c r="AA10" s="212"/>
-      <c r="AB10" s="212"/>
-      <c r="AC10" s="213"/>
+      <c r="B10" s="170"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="173"/>
+      <c r="G10" s="174"/>
+      <c r="H10" s="170"/>
+      <c r="I10" s="171"/>
+      <c r="J10" s="172"/>
+      <c r="K10" s="175"/>
+      <c r="L10" s="176"/>
+      <c r="M10" s="176"/>
+      <c r="N10" s="176"/>
+      <c r="O10" s="176"/>
+      <c r="P10" s="176"/>
+      <c r="Q10" s="176"/>
+      <c r="R10" s="176"/>
+      <c r="S10" s="176"/>
+      <c r="T10" s="176"/>
+      <c r="U10" s="176"/>
+      <c r="V10" s="176"/>
+      <c r="W10" s="177"/>
+      <c r="X10" s="178"/>
+      <c r="Y10" s="179"/>
+      <c r="Z10" s="179"/>
+      <c r="AA10" s="179"/>
+      <c r="AB10" s="179"/>
+      <c r="AC10" s="180"/>
     </row>
     <row r="11" spans="1:30">
-      <c r="B11" s="207"/>
-      <c r="C11" s="203"/>
-      <c r="D11" s="203"/>
-      <c r="E11" s="204"/>
-      <c r="F11" s="205"/>
-      <c r="G11" s="206"/>
-      <c r="H11" s="207"/>
-      <c r="I11" s="203"/>
-      <c r="J11" s="204"/>
-      <c r="K11" s="208"/>
-      <c r="L11" s="209"/>
-      <c r="M11" s="209"/>
-      <c r="N11" s="209"/>
-      <c r="O11" s="209"/>
-      <c r="P11" s="209"/>
-      <c r="Q11" s="209"/>
-      <c r="R11" s="209"/>
-      <c r="S11" s="209"/>
-      <c r="T11" s="209"/>
-      <c r="U11" s="209"/>
-      <c r="V11" s="209"/>
-      <c r="W11" s="210"/>
-      <c r="X11" s="211"/>
-      <c r="Y11" s="212"/>
-      <c r="Z11" s="212"/>
-      <c r="AA11" s="212"/>
-      <c r="AB11" s="212"/>
-      <c r="AC11" s="213"/>
+      <c r="B11" s="170"/>
+      <c r="C11" s="171"/>
+      <c r="D11" s="171"/>
+      <c r="E11" s="172"/>
+      <c r="F11" s="173"/>
+      <c r="G11" s="174"/>
+      <c r="H11" s="170"/>
+      <c r="I11" s="171"/>
+      <c r="J11" s="172"/>
+      <c r="K11" s="175"/>
+      <c r="L11" s="176"/>
+      <c r="M11" s="176"/>
+      <c r="N11" s="176"/>
+      <c r="O11" s="176"/>
+      <c r="P11" s="176"/>
+      <c r="Q11" s="176"/>
+      <c r="R11" s="176"/>
+      <c r="S11" s="176"/>
+      <c r="T11" s="176"/>
+      <c r="U11" s="176"/>
+      <c r="V11" s="176"/>
+      <c r="W11" s="177"/>
+      <c r="X11" s="178"/>
+      <c r="Y11" s="179"/>
+      <c r="Z11" s="179"/>
+      <c r="AA11" s="179"/>
+      <c r="AB11" s="179"/>
+      <c r="AC11" s="180"/>
     </row>
     <row r="12" spans="1:30">
-      <c r="B12" s="207"/>
-      <c r="C12" s="203"/>
-      <c r="D12" s="203"/>
-      <c r="E12" s="204"/>
-      <c r="F12" s="205"/>
-      <c r="G12" s="206"/>
-      <c r="H12" s="207"/>
-      <c r="I12" s="203"/>
-      <c r="J12" s="204"/>
-      <c r="K12" s="208"/>
-      <c r="L12" s="209"/>
-      <c r="M12" s="209"/>
-      <c r="N12" s="209"/>
-      <c r="O12" s="209"/>
-      <c r="P12" s="209"/>
-      <c r="Q12" s="209"/>
-      <c r="R12" s="209"/>
-      <c r="S12" s="209"/>
-      <c r="T12" s="209"/>
-      <c r="U12" s="209"/>
-      <c r="V12" s="209"/>
-      <c r="W12" s="210"/>
-      <c r="X12" s="211"/>
-      <c r="Y12" s="212"/>
-      <c r="Z12" s="212"/>
-      <c r="AA12" s="212"/>
-      <c r="AB12" s="212"/>
-      <c r="AC12" s="213"/>
+      <c r="B12" s="170"/>
+      <c r="C12" s="171"/>
+      <c r="D12" s="171"/>
+      <c r="E12" s="172"/>
+      <c r="F12" s="173"/>
+      <c r="G12" s="174"/>
+      <c r="H12" s="170"/>
+      <c r="I12" s="171"/>
+      <c r="J12" s="172"/>
+      <c r="K12" s="175"/>
+      <c r="L12" s="176"/>
+      <c r="M12" s="176"/>
+      <c r="N12" s="176"/>
+      <c r="O12" s="176"/>
+      <c r="P12" s="176"/>
+      <c r="Q12" s="176"/>
+      <c r="R12" s="176"/>
+      <c r="S12" s="176"/>
+      <c r="T12" s="176"/>
+      <c r="U12" s="176"/>
+      <c r="V12" s="176"/>
+      <c r="W12" s="177"/>
+      <c r="X12" s="178"/>
+      <c r="Y12" s="179"/>
+      <c r="Z12" s="179"/>
+      <c r="AA12" s="179"/>
+      <c r="AB12" s="179"/>
+      <c r="AC12" s="180"/>
     </row>
     <row r="13" spans="1:30" ht="18" customHeight="1"/>
     <row r="14" spans="1:30" ht="18" customHeight="1"/>
@@ -4872,31 +4941,11 @@
     <row r="38" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:W12"/>
-    <mergeCell ref="X12:AC12"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:W10"/>
-    <mergeCell ref="X10:AC10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:W11"/>
-    <mergeCell ref="X11:AC11"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:W8"/>
-    <mergeCell ref="X8:AC8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:W9"/>
-    <mergeCell ref="X9:AC9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AD1"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="A3:C3"/>
@@ -4911,11 +4960,31 @@
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="N2:U2"/>
     <mergeCell ref="V2:X2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:W9"/>
+    <mergeCell ref="X9:AC9"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:W8"/>
+    <mergeCell ref="X8:AC8"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:W11"/>
+    <mergeCell ref="X11:AC11"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:W10"/>
+    <mergeCell ref="X10:AC10"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:W12"/>
+    <mergeCell ref="X12:AC12"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5965,8 +6034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -6020,10 +6089,10 @@
       <c r="C4" s="103" t="s">
         <v>215</v>
       </c>
-      <c r="D4" s="216" t="s">
+      <c r="D4" s="217" t="s">
         <v>218</v>
       </c>
-      <c r="E4" s="216"/>
+      <c r="E4" s="217"/>
       <c r="F4" s="143" t="s">
         <v>216</v>
       </c>
@@ -6041,10 +6110,10 @@
       <c r="C5" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="217" t="s">
+      <c r="D5" s="216" t="s">
         <v>220</v>
       </c>
-      <c r="E5" s="217"/>
+      <c r="E5" s="216"/>
       <c r="F5" s="148" t="s">
         <v>219</v>
       </c>
@@ -6099,24 +6168,28 @@
       <c r="C9" s="143" t="s">
         <v>215</v>
       </c>
-      <c r="D9" s="216" t="s">
+      <c r="D9" s="217" t="s">
         <v>218</v>
       </c>
-      <c r="E9" s="216"/>
+      <c r="E9" s="217"/>
       <c r="F9" s="143" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B10" s="125">
+      <c r="B10" s="249">
         <v>1</v>
       </c>
-      <c r="C10" s="126" t="s">
+      <c r="C10" s="250" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="142"/>
+      <c r="D10" s="251" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" s="251"/>
+      <c r="F10" s="252" t="s">
+        <v>245</v>
+      </c>
       <c r="G10" s="124"/>
       <c r="H10" s="124"/>
     </row>
@@ -6127,9 +6200,9 @@
       <c r="C11" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="215"/>
-      <c r="E11" s="215"/>
-      <c r="F11" s="142"/>
+      <c r="D11" s="247"/>
+      <c r="E11" s="247"/>
+      <c r="F11" s="248"/>
       <c r="G11" s="124"/>
       <c r="H11" s="124"/>
     </row>
@@ -6200,10 +6273,10 @@
       <c r="C18" s="143" t="s">
         <v>215</v>
       </c>
-      <c r="D18" s="216" t="s">
+      <c r="D18" s="217" t="s">
         <v>218</v>
       </c>
-      <c r="E18" s="216"/>
+      <c r="E18" s="217"/>
       <c r="F18" s="143" t="s">
         <v>216</v>
       </c>
@@ -6301,10 +6374,10 @@
       <c r="C27" s="143" t="s">
         <v>215</v>
       </c>
-      <c r="D27" s="216" t="s">
+      <c r="D27" s="217" t="s">
         <v>218</v>
       </c>
-      <c r="E27" s="216"/>
+      <c r="E27" s="217"/>
       <c r="F27" s="143" t="s">
         <v>216</v>
       </c>
@@ -6316,8 +6389,8 @@
       <c r="C28" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="217"/>
-      <c r="E28" s="217"/>
+      <c r="D28" s="216"/>
+      <c r="E28" s="216"/>
       <c r="F28" s="149"/>
       <c r="G28" s="124"/>
       <c r="H28" s="124"/>
@@ -6439,10 +6512,10 @@
       <c r="C40" s="156" t="s">
         <v>215</v>
       </c>
-      <c r="D40" s="216" t="s">
+      <c r="D40" s="217" t="s">
         <v>218</v>
       </c>
-      <c r="E40" s="216"/>
+      <c r="E40" s="217"/>
       <c r="F40" s="156" t="s">
         <v>216</v>
       </c>
@@ -6513,10 +6586,10 @@
       <c r="C49" s="143" t="s">
         <v>215</v>
       </c>
-      <c r="D49" s="216" t="s">
+      <c r="D49" s="217" t="s">
         <v>218</v>
       </c>
-      <c r="E49" s="216"/>
+      <c r="E49" s="217"/>
       <c r="F49" s="143" t="s">
         <v>216</v>
       </c>
@@ -6611,10 +6684,10 @@
       <c r="C60" s="143" t="s">
         <v>215</v>
       </c>
-      <c r="D60" s="216" t="s">
+      <c r="D60" s="217" t="s">
         <v>218</v>
       </c>
-      <c r="E60" s="216"/>
+      <c r="E60" s="217"/>
       <c r="F60" s="143" t="s">
         <v>216</v>
       </c>
@@ -6676,15 +6749,27 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="D65:E65"/>
     <mergeCell ref="D23:E23"/>
@@ -6701,27 +6786,15 @@
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7198,7 +7271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -7284,12 +7357,12 @@
       <c r="C4" s="230" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="231"/>
-      <c r="E4" s="231"/>
-      <c r="F4" s="231"/>
-      <c r="G4" s="231"/>
-      <c r="H4" s="231"/>
-      <c r="I4" s="232"/>
+      <c r="D4" s="239"/>
+      <c r="E4" s="239"/>
+      <c r="F4" s="239"/>
+      <c r="G4" s="239"/>
+      <c r="H4" s="239"/>
+      <c r="I4" s="231"/>
       <c r="J4" s="66"/>
       <c r="K4" s="66"/>
       <c r="L4" s="66"/>
@@ -7305,12 +7378,12 @@
       <c r="C5" s="230" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="231"/>
-      <c r="E5" s="231"/>
-      <c r="F5" s="231"/>
-      <c r="G5" s="231"/>
-      <c r="H5" s="231"/>
-      <c r="I5" s="232"/>
+      <c r="D5" s="239"/>
+      <c r="E5" s="239"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="239"/>
+      <c r="H5" s="239"/>
+      <c r="I5" s="231"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
       <c r="L5" s="66"/>
@@ -7347,12 +7420,12 @@
       <c r="C7" s="230" t="s">
         <v>166</v>
       </c>
-      <c r="D7" s="231"/>
-      <c r="E7" s="231"/>
-      <c r="F7" s="231"/>
-      <c r="G7" s="231"/>
-      <c r="H7" s="231"/>
-      <c r="I7" s="232"/>
+      <c r="D7" s="239"/>
+      <c r="E7" s="239"/>
+      <c r="F7" s="239"/>
+      <c r="G7" s="239"/>
+      <c r="H7" s="239"/>
+      <c r="I7" s="231"/>
       <c r="J7" s="66"/>
       <c r="K7" s="66"/>
       <c r="L7" s="66"/>
@@ -7389,12 +7462,12 @@
       <c r="C9" s="230" t="s">
         <v>212</v>
       </c>
-      <c r="D9" s="231"/>
-      <c r="E9" s="231"/>
-      <c r="F9" s="231"/>
-      <c r="G9" s="231"/>
-      <c r="H9" s="231"/>
-      <c r="I9" s="232"/>
+      <c r="D9" s="239"/>
+      <c r="E9" s="239"/>
+      <c r="F9" s="239"/>
+      <c r="G9" s="239"/>
+      <c r="H9" s="239"/>
+      <c r="I9" s="231"/>
       <c r="J9" s="66"/>
       <c r="K9" s="66"/>
       <c r="L9" s="66"/>
@@ -7457,19 +7530,19 @@
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="66"/>
-      <c r="B13" s="234" t="s">
+      <c r="B13" s="232" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="235"/>
-      <c r="D13" s="235"/>
-      <c r="E13" s="235"/>
-      <c r="F13" s="235"/>
-      <c r="G13" s="235"/>
-      <c r="H13" s="235"/>
-      <c r="I13" s="235"/>
-      <c r="J13" s="235"/>
-      <c r="K13" s="235"/>
-      <c r="L13" s="236"/>
+      <c r="C13" s="233"/>
+      <c r="D13" s="233"/>
+      <c r="E13" s="233"/>
+      <c r="F13" s="233"/>
+      <c r="G13" s="233"/>
+      <c r="H13" s="233"/>
+      <c r="I13" s="233"/>
+      <c r="J13" s="233"/>
+      <c r="K13" s="233"/>
+      <c r="L13" s="234"/>
       <c r="M13" s="66"/>
       <c r="N13" s="66"/>
       <c r="O13" s="66"/>
@@ -7498,11 +7571,11 @@
       <c r="I14" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="J14" s="233" t="s">
+      <c r="J14" s="246" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="233"/>
-      <c r="L14" s="233"/>
+      <c r="K14" s="246"/>
+      <c r="L14" s="246"/>
       <c r="M14" s="66"/>
       <c r="N14" s="66"/>
       <c r="O14" s="66"/>
@@ -7531,11 +7604,11 @@
       <c r="I15" s="81" t="s">
         <v>240</v>
       </c>
-      <c r="J15" s="240" t="s">
+      <c r="J15" s="238" t="s">
         <v>176</v>
       </c>
-      <c r="K15" s="240"/>
-      <c r="L15" s="240"/>
+      <c r="K15" s="238"/>
+      <c r="L15" s="238"/>
       <c r="M15" s="66"/>
       <c r="N15" s="66"/>
       <c r="O15" s="66"/>
@@ -7564,11 +7637,11 @@
       <c r="I16" s="81" t="s">
         <v>241</v>
       </c>
-      <c r="J16" s="240" t="s">
+      <c r="J16" s="238" t="s">
         <v>179</v>
       </c>
-      <c r="K16" s="240"/>
-      <c r="L16" s="240"/>
+      <c r="K16" s="238"/>
+      <c r="L16" s="238"/>
       <c r="M16" s="66"/>
       <c r="N16" s="66"/>
       <c r="O16" s="66"/>
@@ -7633,8 +7706,8 @@
       <c r="J18" s="230" t="s">
         <v>188</v>
       </c>
-      <c r="K18" s="231"/>
-      <c r="L18" s="232"/>
+      <c r="K18" s="239"/>
+      <c r="L18" s="231"/>
       <c r="M18" s="66"/>
       <c r="N18" s="66"/>
       <c r="O18" s="66"/>
@@ -7666,8 +7739,8 @@
       <c r="J19" s="230" t="s">
         <v>192</v>
       </c>
-      <c r="K19" s="231"/>
-      <c r="L19" s="232"/>
+      <c r="K19" s="239"/>
+      <c r="L19" s="231"/>
       <c r="M19" s="66"/>
       <c r="N19" s="66"/>
       <c r="O19" s="66"/>
@@ -7829,11 +7902,11 @@
     </row>
     <row r="29" spans="1:15" s="88" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="69"/>
-      <c r="B29" s="241" t="s">
+      <c r="B29" s="240" t="s">
         <v>183</v>
       </c>
-      <c r="C29" s="241"/>
-      <c r="D29" s="241"/>
+      <c r="C29" s="240"/>
+      <c r="D29" s="240"/>
       <c r="E29" s="86"/>
       <c r="F29" s="87"/>
       <c r="G29" s="86"/>
@@ -7848,12 +7921,12 @@
     </row>
     <row r="30" spans="1:15" s="90" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="89"/>
-      <c r="B30" s="237" t="s">
+      <c r="B30" s="235" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="238"/>
-      <c r="D30" s="238"/>
-      <c r="E30" s="239"/>
+      <c r="C30" s="236"/>
+      <c r="D30" s="236"/>
+      <c r="E30" s="237"/>
       <c r="F30" s="76" t="s">
         <v>132</v>
       </c>
@@ -7945,10 +8018,10 @@
       <c r="A33" s="66"/>
       <c r="B33" s="91"/>
       <c r="C33" s="96"/>
-      <c r="D33" s="231" t="s">
+      <c r="D33" s="239" t="s">
         <v>198</v>
       </c>
-      <c r="E33" s="232"/>
+      <c r="E33" s="231"/>
       <c r="F33" s="78" t="s">
         <v>148</v>
       </c>
@@ -7978,10 +8051,10 @@
       <c r="A34" s="66"/>
       <c r="B34" s="91"/>
       <c r="C34" s="98"/>
-      <c r="D34" s="231" t="s">
+      <c r="D34" s="239" t="s">
         <v>199</v>
       </c>
-      <c r="E34" s="232"/>
+      <c r="E34" s="231"/>
       <c r="F34" s="78" t="s">
         <v>200</v>
       </c>
@@ -8044,10 +8117,10 @@
       <c r="A36" s="66"/>
       <c r="B36" s="91"/>
       <c r="C36" s="96"/>
-      <c r="D36" s="231" t="s">
+      <c r="D36" s="239" t="s">
         <v>202</v>
       </c>
-      <c r="E36" s="232"/>
+      <c r="E36" s="231"/>
       <c r="F36" s="78" t="s">
         <v>204</v>
       </c>
@@ -8077,10 +8150,10 @@
       <c r="A37" s="66"/>
       <c r="B37" s="91"/>
       <c r="C37" s="96"/>
-      <c r="D37" s="245" t="s">
+      <c r="D37" s="244" t="s">
         <v>173</v>
       </c>
-      <c r="E37" s="246"/>
+      <c r="E37" s="245"/>
       <c r="F37" s="78" t="s">
         <v>174</v>
       </c>
@@ -8110,10 +8183,10 @@
       <c r="A38" s="66"/>
       <c r="B38" s="91"/>
       <c r="C38" s="96"/>
-      <c r="D38" s="231" t="s">
+      <c r="D38" s="239" t="s">
         <v>189</v>
       </c>
-      <c r="E38" s="232"/>
+      <c r="E38" s="231"/>
       <c r="F38" s="78" t="s">
         <v>184</v>
       </c>
@@ -8633,10 +8706,10 @@
       <c r="A63" s="66"/>
       <c r="B63" s="91"/>
       <c r="C63" s="96"/>
-      <c r="D63" s="242" t="s">
+      <c r="D63" s="241" t="s">
         <v>198</v>
       </c>
-      <c r="E63" s="232"/>
+      <c r="E63" s="231"/>
       <c r="F63" s="78" t="s">
         <v>148</v>
       </c>
@@ -8666,10 +8739,10 @@
       <c r="A64" s="66"/>
       <c r="B64" s="91"/>
       <c r="C64" s="96"/>
-      <c r="D64" s="242" t="s">
+      <c r="D64" s="241" t="s">
         <v>0</v>
       </c>
-      <c r="E64" s="243"/>
+      <c r="E64" s="242"/>
       <c r="F64" s="150" t="s">
         <v>221</v>
       </c>
@@ -8699,10 +8772,10 @@
       <c r="A65" s="66"/>
       <c r="B65" s="91"/>
       <c r="C65" s="96"/>
-      <c r="D65" s="244" t="s">
+      <c r="D65" s="243" t="s">
         <v>226</v>
       </c>
-      <c r="E65" s="243"/>
+      <c r="E65" s="242"/>
       <c r="F65" s="150" t="s">
         <v>224</v>
       </c>
@@ -8797,7 +8870,7 @@
       <c r="B68" s="97"/>
       <c r="C68" s="98"/>
       <c r="D68" s="230"/>
-      <c r="E68" s="232"/>
+      <c r="E68" s="231"/>
       <c r="F68" s="78"/>
       <c r="G68" s="80"/>
       <c r="H68" s="80"/>
@@ -9193,6 +9266,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B30:E30"/>
@@ -9209,11 +9287,6 @@
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <phoneticPr fontId="14"/>
   <hyperlinks>

</xml_diff>